<commit_message>
added data science method with pandas dataframe
</commit_message>
<xml_diff>
--- a/resources/SAS test.xlsx
+++ b/resources/SAS test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonty/projects/Finance/bond-calculator/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914B7E53-1913-CC4B-9AB7-6C08C3AA9E4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF65D90-A20D-4944-94D9-D054E0053BE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18820" activeTab="1" xr2:uid="{A9929AB1-C006-EC48-9772-E431D1BA52C8}"/>
   </bookViews>
@@ -395,8 +395,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{543B0A36-A2F6-D547-A2B3-2710BBC76960}" name="Table5" displayName="Table5" ref="O1:S7" totalsRowShown="0">
-  <autoFilter ref="O1:S7" xr:uid="{543B0A36-A2F6-D547-A2B3-2710BBC76960}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{543B0A36-A2F6-D547-A2B3-2710BBC76960}" name="Table5" displayName="Table5" ref="O1:S6" totalsRowShown="0">
+  <autoFilter ref="O1:S6" xr:uid="{543B0A36-A2F6-D547-A2B3-2710BBC76960}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{15BC2723-93B1-1141-94E1-EF1C5DAD39C3}" name="Value" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{663494FB-6A22-AA46-8F7F-2278EB9E6055}" name="Interest added" dataDxfId="2"/>
@@ -878,7 +878,7 @@
   <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1197,6 +1197,7 @@
         <f t="shared" si="2"/>
         <v>3631.763251807246</v>
       </c>
+      <c r="O8" s="7"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="H9" s="9">
@@ -1217,7 +1218,6 @@
         <f t="shared" si="2"/>
         <v>2490.9890469156808</v>
       </c>
-      <c r="O9" s="7"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="H10" s="9">

</xml_diff>